<commit_message>
Military and suicide data has been updated
</commit_message>
<xml_diff>
--- a/app/countries/management/commands/data/reserve_currencies.xlsx
+++ b/app/countries/management/commands/data/reserve_currencies.xlsx
@@ -20,54 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Claims in U.S. dollars</t>
   </si>
   <si>
-    <t xml:space="preserve">6652.36</t>
-  </si>
-  <si>
     <t xml:space="preserve">Claims in euro</t>
   </si>
   <si>
-    <t xml:space="preserve">2208.93</t>
-  </si>
-  <si>
     <t xml:space="preserve">Claims in Chinese renminbi</t>
   </si>
   <si>
-    <t xml:space="preserve">322.38</t>
-  </si>
-  <si>
     <t xml:space="preserve">Claims in Japanese yen</t>
   </si>
   <si>
-    <t xml:space="preserve">578.52</t>
-  </si>
-  <si>
     <t xml:space="preserve">Claims in pounds sterling</t>
   </si>
   <si>
-    <t xml:space="preserve">545.08</t>
-  </si>
-  <si>
     <t xml:space="preserve">Claims in Australian dollars</t>
   </si>
   <si>
-    <t xml:space="preserve">210.01</t>
-  </si>
-  <si>
     <t xml:space="preserve">Claims in Canadian dollars</t>
   </si>
   <si>
-    <t xml:space="preserve">278.18</t>
-  </si>
-  <si>
     <t xml:space="preserve">Claims in Swiss francs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27.62</t>
   </si>
 </sst>
 </file>
@@ -176,7 +152,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -188,64 +164,64 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
+      <c r="B1" s="2" t="n">
+        <v>6441.65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>2117.94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>297.79</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>566.43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>497.33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>206.26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>264.15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>25.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>